<commit_message>
Redo single layer networks with other category recoded
</commit_message>
<xml_diff>
--- a/CurrentData/Raw Edgelists_Excel/SLR_raw_concerns.xlsx
+++ b/CurrentData/Raw Edgelists_Excel/SLR_raw_concerns.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1979" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1979" uniqueCount="22">
   <si>
     <t>Concern 1</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Erosion</t>
-  </si>
-  <si>
-    <t>FirstOther</t>
   </si>
   <si>
     <t>Public Health</t>
@@ -413,8 +410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C869"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A467" workbookViewId="0">
+      <selection activeCell="G471" sqref="G471"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,7 +597,7 @@
         <v>3</v>
       </c>
       <c r="B128" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C128" t="s">
         <v>4</v>
@@ -633,7 +630,7 @@
         <v>5</v>
       </c>
       <c r="B131" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C131" t="s">
         <v>4</v>
@@ -655,7 +652,7 @@
         <v>4</v>
       </c>
       <c r="B133" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C133" t="s">
         <v>6</v>
@@ -798,7 +795,7 @@
         <v>5</v>
       </c>
       <c r="B147" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C147" t="s">
         <v>3</v>
@@ -886,7 +883,7 @@
         <v>6</v>
       </c>
       <c r="C157" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -897,7 +894,7 @@
         <v>4</v>
       </c>
       <c r="C158" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -930,7 +927,7 @@
         <v>6</v>
       </c>
       <c r="C161" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -960,7 +957,7 @@
         <v>4</v>
       </c>
       <c r="B164" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C164" t="s">
         <v>5</v>
@@ -971,7 +968,7 @@
         <v>4</v>
       </c>
       <c r="B165" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C165" t="s">
         <v>6</v>
@@ -982,7 +979,7 @@
         <v>5</v>
       </c>
       <c r="B167" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C167" t="s">
         <v>7</v>
@@ -1136,7 +1133,7 @@
         <v>7</v>
       </c>
       <c r="B181" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C181" t="s">
         <v>4</v>
@@ -1169,7 +1166,7 @@
         <v>5</v>
       </c>
       <c r="B185" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C185" t="s">
         <v>4</v>
@@ -1235,7 +1232,7 @@
         <v>6</v>
       </c>
       <c r="B191" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C191" t="s">
         <v>4</v>
@@ -1301,7 +1298,7 @@
         <v>5</v>
       </c>
       <c r="B197" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C197" t="s">
         <v>7</v>
@@ -1378,7 +1375,7 @@
         <v>7</v>
       </c>
       <c r="B204" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C204" t="s">
         <v>3</v>
@@ -1414,7 +1411,7 @@
         <v>4</v>
       </c>
       <c r="C208" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -1565,7 +1562,7 @@
         <v>6</v>
       </c>
       <c r="B222" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C222" t="s">
         <v>4</v>
@@ -1631,7 +1628,7 @@
         <v>5</v>
       </c>
       <c r="B228" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C228" t="s">
         <v>3</v>
@@ -1642,7 +1639,7 @@
         <v>5</v>
       </c>
       <c r="B229" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C229" t="s">
         <v>12</v>
@@ -1650,10 +1647,10 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B230" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C230" t="s">
         <v>5</v>
@@ -1708,7 +1705,7 @@
         <v>5</v>
       </c>
       <c r="B235" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C235" t="s">
         <v>4</v>
@@ -1752,7 +1749,7 @@
         <v>4</v>
       </c>
       <c r="B240" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C240" t="s">
         <v>5</v>
@@ -1785,10 +1782,10 @@
         <v>5</v>
       </c>
       <c r="B243" t="s">
+        <v>13</v>
+      </c>
+      <c r="C243" t="s">
         <v>14</v>
-      </c>
-      <c r="C243" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -1799,7 +1796,7 @@
         <v>9</v>
       </c>
       <c r="C244" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -1829,7 +1826,7 @@
         <v>7</v>
       </c>
       <c r="B247" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C247" t="s">
         <v>12</v>
@@ -1991,7 +1988,7 @@
         <v>7</v>
       </c>
       <c r="B263" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C263" t="s">
         <v>12</v>
@@ -2046,7 +2043,7 @@
         <v>4</v>
       </c>
       <c r="B268" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C268" t="s">
         <v>7</v>
@@ -2057,7 +2054,7 @@
         <v>12</v>
       </c>
       <c r="B269" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C269" t="s">
         <v>7</v>
@@ -2123,7 +2120,7 @@
         <v>3</v>
       </c>
       <c r="B275" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C275" t="s">
         <v>4</v>
@@ -2134,7 +2131,7 @@
         <v>7</v>
       </c>
       <c r="B276" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C276" t="s">
         <v>6</v>
@@ -2156,7 +2153,7 @@
         <v>6</v>
       </c>
       <c r="B278" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C278" t="s">
         <v>5</v>
@@ -2178,7 +2175,7 @@
         <v>6</v>
       </c>
       <c r="B280" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C280" t="s">
         <v>10</v>
@@ -2214,7 +2211,7 @@
         <v>7</v>
       </c>
       <c r="C283" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -2321,7 +2318,7 @@
         <v>5</v>
       </c>
       <c r="B293" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C293" t="s">
         <v>4</v>
@@ -2362,7 +2359,7 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B297" t="s">
         <v>6</v>
@@ -2431,7 +2428,7 @@
         <v>7</v>
       </c>
       <c r="B303" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C303" t="s">
         <v>5</v>
@@ -2467,7 +2464,7 @@
         <v>6</v>
       </c>
       <c r="C307" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
@@ -2508,7 +2505,7 @@
         <v>5</v>
       </c>
       <c r="B312" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C312" t="s">
         <v>4</v>
@@ -2571,7 +2568,7 @@
         <v>5</v>
       </c>
       <c r="B318" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C318" t="s">
         <v>7</v>
@@ -2802,7 +2799,7 @@
         <v>4</v>
       </c>
       <c r="B341" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C341" t="s">
         <v>8</v>
@@ -2824,7 +2821,7 @@
         <v>5</v>
       </c>
       <c r="B343" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C343" t="s">
         <v>3</v>
@@ -2835,7 +2832,7 @@
         <v>3</v>
       </c>
       <c r="B344" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C344" t="s">
         <v>5</v>
@@ -2846,7 +2843,7 @@
         <v>5</v>
       </c>
       <c r="B345" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C345" t="s">
         <v>11</v>
@@ -2931,7 +2928,7 @@
         <v>6</v>
       </c>
       <c r="B353" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C353" t="s">
         <v>4</v>
@@ -2964,7 +2961,7 @@
         <v>7</v>
       </c>
       <c r="B356" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C356" t="s">
         <v>3</v>
@@ -3005,7 +3002,7 @@
         <v>7</v>
       </c>
       <c r="B360" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C360" t="s">
         <v>4</v>
@@ -3184,7 +3181,7 @@
         <v>12</v>
       </c>
       <c r="C376" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
@@ -3255,7 +3252,7 @@
         <v>4</v>
       </c>
       <c r="C383" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
@@ -3381,10 +3378,10 @@
         <v>4</v>
       </c>
       <c r="B396" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C396" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
@@ -3406,7 +3403,7 @@
         <v>8</v>
       </c>
       <c r="C398" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
@@ -3428,7 +3425,7 @@
         <v>9</v>
       </c>
       <c r="C400" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.25">
@@ -3447,7 +3444,7 @@
         <v>5</v>
       </c>
       <c r="B402" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C402" t="s">
         <v>7</v>
@@ -3491,7 +3488,7 @@
         <v>7</v>
       </c>
       <c r="B407" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C407" t="s">
         <v>6</v>
@@ -3513,7 +3510,7 @@
         <v>6</v>
       </c>
       <c r="B411" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C411" t="s">
         <v>12</v>
@@ -3557,7 +3554,7 @@
         <v>6</v>
       </c>
       <c r="B415" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C415" t="s">
         <v>8</v>
@@ -3653,7 +3650,7 @@
         <v>12</v>
       </c>
       <c r="B426" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C426" t="s">
         <v>6</v>
@@ -3664,7 +3661,7 @@
         <v>5</v>
       </c>
       <c r="B427" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C427" t="s">
         <v>7</v>
@@ -3686,7 +3683,7 @@
         <v>7</v>
       </c>
       <c r="B429" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C429" t="s">
         <v>6</v>
@@ -3719,7 +3716,7 @@
         <v>3</v>
       </c>
       <c r="B432" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C432" t="s">
         <v>8</v>
@@ -3752,7 +3749,7 @@
         <v>5</v>
       </c>
       <c r="B435" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C435" t="s">
         <v>4</v>
@@ -3909,7 +3906,7 @@
         <v>4</v>
       </c>
       <c r="C453" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="454" spans="1:3" x14ac:dyDescent="0.25">
@@ -3980,7 +3977,7 @@
         <v>4</v>
       </c>
       <c r="C460" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.25">
@@ -3993,7 +3990,7 @@
         <v>5</v>
       </c>
       <c r="B462" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C462" t="s">
         <v>7</v>
@@ -4018,7 +4015,7 @@
         <v>12</v>
       </c>
       <c r="C464" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="465" spans="1:3" x14ac:dyDescent="0.25">
@@ -4037,7 +4034,7 @@
         <v>3</v>
       </c>
       <c r="B466" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C466" t="s">
         <v>7</v>
@@ -4048,7 +4045,7 @@
         <v>10</v>
       </c>
       <c r="B467" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C467" t="s">
         <v>7</v>
@@ -4103,7 +4100,7 @@
         <v>4</v>
       </c>
       <c r="B472" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C472" t="s">
         <v>8</v>
@@ -4224,7 +4221,7 @@
         <v>4</v>
       </c>
       <c r="B483" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C483" t="s">
         <v>3</v>
@@ -4246,7 +4243,7 @@
         <v>5</v>
       </c>
       <c r="B485" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C485" t="s">
         <v>4</v>
@@ -4378,7 +4375,7 @@
         <v>7</v>
       </c>
       <c r="C498" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="499" spans="1:3" x14ac:dyDescent="0.25">
@@ -4386,10 +4383,10 @@
         <v>5</v>
       </c>
       <c r="B499" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C499" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="500" spans="1:3" x14ac:dyDescent="0.25">
@@ -4408,10 +4405,10 @@
         <v>3</v>
       </c>
       <c r="B501" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C501" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.25">
@@ -4455,7 +4452,7 @@
         <v>3</v>
       </c>
       <c r="C505" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="506" spans="1:3" x14ac:dyDescent="0.25">
@@ -4477,7 +4474,7 @@
         <v>6</v>
       </c>
       <c r="C507" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="508" spans="1:3" x14ac:dyDescent="0.25">
@@ -4518,7 +4515,7 @@
         <v>3</v>
       </c>
       <c r="C511" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="512" spans="1:3" x14ac:dyDescent="0.25">
@@ -4632,7 +4629,7 @@
         <v>5</v>
       </c>
       <c r="B525" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C525" t="s">
         <v>7</v>
@@ -4756,7 +4753,7 @@
         <v>4</v>
       </c>
       <c r="C536" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="537" spans="1:3" x14ac:dyDescent="0.25">
@@ -4808,7 +4805,7 @@
         <v>7</v>
       </c>
       <c r="B541" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C541" t="s">
         <v>5</v>
@@ -4874,7 +4871,7 @@
         <v>7</v>
       </c>
       <c r="B547" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C547" t="s">
         <v>4</v>
@@ -4885,7 +4882,7 @@
         <v>3</v>
       </c>
       <c r="B548" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C548" t="s">
         <v>6</v>
@@ -4921,7 +4918,7 @@
         <v>7</v>
       </c>
       <c r="C551" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="552" spans="1:3" x14ac:dyDescent="0.25">
@@ -4976,7 +4973,7 @@
         <v>12</v>
       </c>
       <c r="C556" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="557" spans="1:3" x14ac:dyDescent="0.25">
@@ -4984,7 +4981,7 @@
         <v>6</v>
       </c>
       <c r="B557" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C557" t="s">
         <v>4</v>
@@ -5028,7 +5025,7 @@
         <v>5</v>
       </c>
       <c r="B561" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C561" t="s">
         <v>4</v>
@@ -5050,7 +5047,7 @@
         <v>5</v>
       </c>
       <c r="B564" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C564" t="s">
         <v>4</v>
@@ -5179,7 +5176,7 @@
         <v>7</v>
       </c>
       <c r="B577" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C577" t="s">
         <v>4</v>
@@ -5300,7 +5297,7 @@
         <v>5</v>
       </c>
       <c r="B588" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C588" t="s">
         <v>7</v>
@@ -5311,7 +5308,7 @@
         <v>3</v>
       </c>
       <c r="B589" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C589" t="s">
         <v>7</v>
@@ -5344,7 +5341,7 @@
         <v>5</v>
       </c>
       <c r="B592" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C592" t="s">
         <v>7</v>
@@ -5388,7 +5385,7 @@
         <v>6</v>
       </c>
       <c r="B596" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C596" t="s">
         <v>4</v>
@@ -5424,7 +5421,7 @@
         <v>4</v>
       </c>
       <c r="C599" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="600" spans="1:3" x14ac:dyDescent="0.25">
@@ -5495,7 +5492,7 @@
     </row>
     <row r="606" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A606" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B606" t="s">
         <v>12</v>
@@ -5635,7 +5632,7 @@
     </row>
     <row r="620" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B620" t="s">
         <v>12</v>
@@ -5660,7 +5657,7 @@
         <v>7</v>
       </c>
       <c r="B622" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C622" t="s">
         <v>5</v>
@@ -5704,7 +5701,7 @@
         <v>12</v>
       </c>
       <c r="B627" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C627" t="s">
         <v>7</v>
@@ -5737,7 +5734,7 @@
         <v>3</v>
       </c>
       <c r="B631" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C631" t="s">
         <v>6</v>
@@ -5814,7 +5811,7 @@
         <v>3</v>
       </c>
       <c r="B638" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C638" t="s">
         <v>5</v>
@@ -5976,7 +5973,7 @@
         <v>7</v>
       </c>
       <c r="B654" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C654" t="s">
         <v>5</v>
@@ -6099,7 +6096,7 @@
         <v>6</v>
       </c>
       <c r="C666" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="667" spans="1:3" x14ac:dyDescent="0.25">
@@ -6181,7 +6178,7 @@
     </row>
     <row r="674" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="675" spans="1:3" x14ac:dyDescent="0.25">
@@ -6189,7 +6186,7 @@
         <v>5</v>
       </c>
       <c r="B675" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C675" t="s">
         <v>4</v>
@@ -6203,29 +6200,29 @@
         <v>8</v>
       </c>
       <c r="C676" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="677" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B677" t="s">
         <v>4</v>
       </c>
       <c r="C677" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="678" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B678" t="s">
         <v>8</v>
       </c>
       <c r="C678" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="679" spans="1:3" x14ac:dyDescent="0.25">
@@ -6260,7 +6257,7 @@
     </row>
     <row r="682" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B682" t="s">
         <v>6</v>
@@ -6282,7 +6279,7 @@
         <v>12</v>
       </c>
       <c r="C684" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="686" spans="1:3" x14ac:dyDescent="0.25">
@@ -6312,7 +6309,7 @@
         <v>5</v>
       </c>
       <c r="B688" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C688" t="s">
         <v>4</v>
@@ -6323,7 +6320,7 @@
         <v>5</v>
       </c>
       <c r="B689" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C689" t="s">
         <v>4</v>
@@ -6433,10 +6430,10 @@
         <v>4</v>
       </c>
       <c r="B699" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C699" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="700" spans="1:3" x14ac:dyDescent="0.25">
@@ -6455,7 +6452,7 @@
         <v>6</v>
       </c>
       <c r="B701" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C701" t="s">
         <v>3</v>
@@ -6488,7 +6485,7 @@
         <v>5</v>
       </c>
       <c r="B705" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C705" t="s">
         <v>3</v>
@@ -6499,7 +6496,7 @@
         <v>5</v>
       </c>
       <c r="B706" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C706" t="s">
         <v>9</v>
@@ -6623,7 +6620,7 @@
         <v>7</v>
       </c>
       <c r="C717" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="718" spans="1:3" x14ac:dyDescent="0.25">
@@ -6631,7 +6628,7 @@
         <v>3</v>
       </c>
       <c r="B718" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C718" t="s">
         <v>6</v>
@@ -6686,7 +6683,7 @@
         <v>7</v>
       </c>
       <c r="B723" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C723" t="s">
         <v>4</v>
@@ -6719,7 +6716,7 @@
         <v>5</v>
       </c>
       <c r="B726" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C726" t="s">
         <v>4</v>
@@ -6744,7 +6741,7 @@
         <v>6</v>
       </c>
       <c r="C729" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="730" spans="1:3" x14ac:dyDescent="0.25">
@@ -6754,7 +6751,7 @@
     </row>
     <row r="731" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B731" t="s">
         <v>8</v>
@@ -6768,10 +6765,10 @@
         <v>5</v>
       </c>
       <c r="B732" t="s">
+        <v>13</v>
+      </c>
+      <c r="C732" t="s">
         <v>14</v>
-      </c>
-      <c r="C732" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="733" spans="1:3" x14ac:dyDescent="0.25">
@@ -6815,7 +6812,7 @@
         <v>6</v>
       </c>
       <c r="C737" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="738" spans="1:3" x14ac:dyDescent="0.25">
@@ -6834,7 +6831,7 @@
         <v>7</v>
       </c>
       <c r="B739" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C739" t="s">
         <v>4</v>
@@ -6867,7 +6864,7 @@
         <v>5</v>
       </c>
       <c r="B742" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C742" t="s">
         <v>6</v>
@@ -6903,7 +6900,7 @@
         <v>4</v>
       </c>
       <c r="C748" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="749" spans="1:3" x14ac:dyDescent="0.25">
@@ -6974,7 +6971,7 @@
         <v>5</v>
       </c>
       <c r="B757" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C757" t="s">
         <v>3</v>
@@ -6996,7 +6993,7 @@
         <v>7</v>
       </c>
       <c r="B760" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C760" t="s">
         <v>4</v>
@@ -7018,7 +7015,7 @@
         <v>5</v>
       </c>
       <c r="B762" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C762" t="s">
         <v>4</v>
@@ -7051,7 +7048,7 @@
         <v>5</v>
       </c>
       <c r="B765" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C765" t="s">
         <v>4</v>
@@ -7117,7 +7114,7 @@
         <v>3</v>
       </c>
       <c r="B771" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C771" t="s">
         <v>4</v>
@@ -7210,7 +7207,7 @@
         <v>3</v>
       </c>
       <c r="B780" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C780" t="s">
         <v>4</v>
@@ -7259,7 +7256,7 @@
         <v>4</v>
       </c>
       <c r="B786" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C786" t="s">
         <v>3</v>
@@ -7314,7 +7311,7 @@
         <v>7</v>
       </c>
       <c r="B792" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C792" t="s">
         <v>4</v>
@@ -7328,7 +7325,7 @@
         <v>4</v>
       </c>
       <c r="C793" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="794" spans="1:3" x14ac:dyDescent="0.25">
@@ -7336,7 +7333,7 @@
         <v>6</v>
       </c>
       <c r="B794" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C794" t="s">
         <v>4</v>
@@ -7432,7 +7429,7 @@
         <v>5</v>
       </c>
       <c r="B804" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C804" s="1" t="s">
         <v>7</v>
@@ -7558,7 +7555,7 @@
         <v>4</v>
       </c>
       <c r="B826" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C826" t="s">
         <v>8</v>
@@ -7602,7 +7599,7 @@
         <v>7</v>
       </c>
       <c r="B837" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="839" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>